<commit_message>
aggiunto codice per ppo continual
- aggiunto codice per ppo continual
</commit_message>
<xml_diff>
--- a/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
+++ b/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,15 +444,23 @@
           <t>ins_max</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>timesteps</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>adult#009</t>
+          <t>adult#001</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunti script test finali e script per ws
- aggiunti script finali per single ppo, double ppo e ablation study
- aggiunti stessi script per ws
</commit_message>
<xml_diff>
--- a/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
+++ b/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
@@ -453,14 +453,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>adult#001</t>
+          <t>adult#004</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.09</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>2400</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunto codice per continual learning
Aggiunto codice per continual learning
</commit_message>
<xml_diff>
--- a/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
+++ b/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
@@ -453,14 +453,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>adult#004</t>
+          <t>adult#001</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>0.06</v>
       </c>
       <c r="C2" t="n">
-        <v>100000</v>
+        <v>16384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sistema dataframe continual learning
- continual learning con sistema per raccogliere dati
- data su cui basare il salvataggio finale del dataframe DA SISTEMARE
</commit_message>
<xml_diff>
--- a/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
+++ b/Simulazioni_RL/Risultati/Strategy/paz_cap.xlsx
@@ -453,14 +453,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>adult#001</t>
+          <t>adult#009</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="C2" t="n">
-        <v>16384</v>
+        <v>2048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>